<commit_message>
Add migration file for client_activity table and update related Excel templates
- Created a new migration file (Migration/111) containing the schema for the client_activity table, including its columns and relationships with groups, client_units, and years.
- Updated the Excel report file for 2025 to reflect the latest changes in the database schema.
- Modified the empty template Excel file to ensure it aligns with the new structure and requirements.
</commit_message>
<xml_diff>
--- a/cod_Migration/reports/Анлиз_2025_1-5.xlsx
+++ b/cod_Migration/reports/Анлиз_2025_1-5.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
-  <si>
-    <t>Created by LibXL trial version 4.6.0. Please buy the LibXL full version for removing this message.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Группа</t>
   </si>
@@ -125,7 +122,7 @@
     <t>Повторно основные</t>
   </si>
   <si>
-    <t>Постоянные основные</t>
+    <t>Постоянные</t>
   </si>
   <si>
     <t>Всего</t>
@@ -326,18 +323,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1246,7 +1237,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1270,16 +1261,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1288,135 +1279,138 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
@@ -1437,10 +1431,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1461,10 +1455,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
@@ -1473,16 +1467,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
@@ -1503,37 +1497,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
@@ -1566,16 +1560,16 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1593,46 +1587,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
@@ -1653,25 +1647,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
@@ -1692,19 +1686,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2032,7 +2026,7 @@
   <dimension ref="A1:IV36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -2045,1164 +2039,1160 @@
     <col min="11" max="11" width="34.2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1" spans="1:256">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="1" ht="20" customHeight="1" spans="1:256">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="2"/>
+      <c r="CC1" s="2"/>
+      <c r="CD1" s="2"/>
+      <c r="CE1" s="2"/>
+      <c r="CF1" s="2"/>
+      <c r="CG1" s="2"/>
+      <c r="CH1" s="2"/>
+      <c r="CI1" s="2"/>
+      <c r="CJ1" s="2"/>
+      <c r="CK1" s="2"/>
+      <c r="CL1" s="2"/>
+      <c r="CM1" s="2"/>
+      <c r="CN1" s="2"/>
+      <c r="CO1" s="2"/>
+      <c r="CP1" s="2"/>
+      <c r="CQ1" s="2"/>
+      <c r="CR1" s="2"/>
+      <c r="CS1" s="2"/>
+      <c r="CT1" s="2"/>
+      <c r="CU1" s="2"/>
+      <c r="CV1" s="2"/>
+      <c r="CW1" s="2"/>
+      <c r="CX1" s="2"/>
+      <c r="CY1" s="2"/>
+      <c r="CZ1" s="2"/>
+      <c r="DA1" s="2"/>
+      <c r="DB1" s="2"/>
+      <c r="DC1" s="2"/>
+      <c r="DD1" s="2"/>
+      <c r="DE1" s="2"/>
+      <c r="DF1" s="2"/>
+      <c r="DG1" s="2"/>
+      <c r="DH1" s="2"/>
+      <c r="DI1" s="2"/>
+      <c r="DJ1" s="2"/>
+      <c r="DK1" s="2"/>
+      <c r="DL1" s="2"/>
+      <c r="DM1" s="2"/>
+      <c r="DN1" s="2"/>
+      <c r="DO1" s="2"/>
+      <c r="DP1" s="2"/>
+      <c r="DQ1" s="2"/>
+      <c r="DR1" s="2"/>
+      <c r="DS1" s="2"/>
+      <c r="DT1" s="2"/>
+      <c r="DU1" s="2"/>
+      <c r="DV1" s="2"/>
+      <c r="DW1" s="2"/>
+      <c r="DX1" s="2"/>
+      <c r="DY1" s="2"/>
+      <c r="DZ1" s="2"/>
+      <c r="EA1" s="2"/>
+      <c r="EB1" s="2"/>
+      <c r="EC1" s="2"/>
+      <c r="ED1" s="2"/>
+      <c r="EE1" s="2"/>
+      <c r="EF1" s="2"/>
+      <c r="EG1" s="2"/>
+      <c r="EH1" s="2"/>
+      <c r="EI1" s="2"/>
+      <c r="EJ1" s="2"/>
+      <c r="EK1" s="2"/>
+      <c r="EL1" s="2"/>
+      <c r="EM1" s="2"/>
+      <c r="EN1" s="2"/>
+      <c r="EO1" s="2"/>
+      <c r="EP1" s="2"/>
+      <c r="EQ1" s="2"/>
+      <c r="ER1" s="2"/>
+      <c r="ES1" s="2"/>
+      <c r="ET1" s="2"/>
+      <c r="EU1" s="2"/>
+      <c r="EV1" s="2"/>
+      <c r="EW1" s="2"/>
+      <c r="EX1" s="2"/>
+      <c r="EY1" s="2"/>
+      <c r="EZ1" s="2"/>
+      <c r="FA1" s="2"/>
+      <c r="FB1" s="2"/>
+      <c r="FC1" s="2"/>
+      <c r="FD1" s="2"/>
+      <c r="FE1" s="2"/>
+      <c r="FF1" s="2"/>
+      <c r="FG1" s="2"/>
+      <c r="FH1" s="2"/>
+      <c r="FI1" s="2"/>
+      <c r="FJ1" s="2"/>
+      <c r="FK1" s="2"/>
+      <c r="FL1" s="2"/>
+      <c r="FM1" s="2"/>
+      <c r="FN1" s="2"/>
+      <c r="FO1" s="2"/>
+      <c r="FP1" s="2"/>
+      <c r="FQ1" s="2"/>
+      <c r="FR1" s="2"/>
+      <c r="FS1" s="2"/>
+      <c r="FT1" s="2"/>
+      <c r="FU1" s="2"/>
+      <c r="FV1" s="2"/>
+      <c r="FW1" s="2"/>
+      <c r="FX1" s="2"/>
+      <c r="FY1" s="2"/>
+      <c r="FZ1" s="2"/>
+      <c r="GA1" s="2"/>
+      <c r="GB1" s="2"/>
+      <c r="GC1" s="2"/>
+      <c r="GD1" s="2"/>
+      <c r="GE1" s="2"/>
+      <c r="GF1" s="2"/>
+      <c r="GG1" s="2"/>
+      <c r="GH1" s="2"/>
+      <c r="GI1" s="2"/>
+      <c r="GJ1" s="2"/>
+      <c r="GK1" s="2"/>
+      <c r="GL1" s="2"/>
+      <c r="GM1" s="2"/>
+      <c r="GN1" s="2"/>
+      <c r="GO1" s="2"/>
+      <c r="GP1" s="2"/>
+      <c r="GQ1" s="2"/>
+      <c r="GR1" s="2"/>
+      <c r="GS1" s="2"/>
+      <c r="GT1" s="2"/>
+      <c r="GU1" s="2"/>
+      <c r="GV1" s="2"/>
+      <c r="GW1" s="2"/>
+      <c r="GX1" s="2"/>
+      <c r="GY1" s="2"/>
+      <c r="GZ1" s="2"/>
+      <c r="HA1" s="2"/>
+      <c r="HB1" s="2"/>
+      <c r="HC1" s="2"/>
+      <c r="HD1" s="2"/>
+      <c r="HE1" s="2"/>
+      <c r="HF1" s="2"/>
+      <c r="HG1" s="2"/>
+      <c r="HH1" s="2"/>
+      <c r="HI1" s="2"/>
+      <c r="HJ1" s="2"/>
+      <c r="HK1" s="2"/>
+      <c r="HL1" s="2"/>
+      <c r="HM1" s="2"/>
+      <c r="HN1" s="2"/>
+      <c r="HO1" s="2"/>
+      <c r="HP1" s="2"/>
+      <c r="HQ1" s="2"/>
+      <c r="HR1" s="2"/>
+      <c r="HS1" s="2"/>
+      <c r="HT1" s="2"/>
+      <c r="HU1" s="2"/>
+      <c r="HV1" s="2"/>
+      <c r="HW1" s="2"/>
+      <c r="HX1" s="2"/>
+      <c r="HY1" s="2"/>
+      <c r="HZ1" s="2"/>
+      <c r="IA1" s="2"/>
+      <c r="IB1" s="2"/>
+      <c r="IC1" s="2"/>
+      <c r="ID1" s="2"/>
+      <c r="IE1" s="2"/>
+      <c r="IF1" s="2"/>
+      <c r="IG1" s="2"/>
+      <c r="IH1" s="2"/>
+      <c r="II1" s="2"/>
+      <c r="IJ1" s="2"/>
+      <c r="IK1" s="2"/>
+      <c r="IL1" s="2"/>
+      <c r="IM1" s="2"/>
+      <c r="IN1" s="2"/>
+      <c r="IO1" s="2"/>
+      <c r="IP1" s="2"/>
+      <c r="IQ1" s="2"/>
+      <c r="IR1" s="2"/>
+      <c r="IS1" s="2"/>
+      <c r="IT1" s="2"/>
+      <c r="IU1" s="2"/>
+      <c r="IV1" s="2"/>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
-      <c r="BS1" s="1"/>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1"/>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-      <c r="CA1" s="1"/>
-      <c r="CB1" s="1"/>
-      <c r="CC1" s="1"/>
-      <c r="CD1" s="1"/>
-      <c r="CE1" s="1"/>
-      <c r="CF1" s="1"/>
-      <c r="CG1" s="1"/>
-      <c r="CH1" s="1"/>
-      <c r="CI1" s="1"/>
-      <c r="CJ1" s="1"/>
-      <c r="CK1" s="1"/>
-      <c r="CL1" s="1"/>
-      <c r="CM1" s="1"/>
-      <c r="CN1" s="1"/>
-      <c r="CO1" s="1"/>
-      <c r="CP1" s="1"/>
-      <c r="CQ1" s="1"/>
-      <c r="CR1" s="1"/>
-      <c r="CS1" s="1"/>
-      <c r="CT1" s="1"/>
-      <c r="CU1" s="1"/>
-      <c r="CV1" s="1"/>
-      <c r="CW1" s="1"/>
-      <c r="CX1" s="1"/>
-      <c r="CY1" s="1"/>
-      <c r="CZ1" s="1"/>
-      <c r="DA1" s="1"/>
-      <c r="DB1" s="1"/>
-      <c r="DC1" s="1"/>
-      <c r="DD1" s="1"/>
-      <c r="DE1" s="1"/>
-      <c r="DF1" s="1"/>
-      <c r="DG1" s="1"/>
-      <c r="DH1" s="1"/>
-      <c r="DI1" s="1"/>
-      <c r="DJ1" s="1"/>
-      <c r="DK1" s="1"/>
-      <c r="DL1" s="1"/>
-      <c r="DM1" s="1"/>
-      <c r="DN1" s="1"/>
-      <c r="DO1" s="1"/>
-      <c r="DP1" s="1"/>
-      <c r="DQ1" s="1"/>
-      <c r="DR1" s="1"/>
-      <c r="DS1" s="1"/>
-      <c r="DT1" s="1"/>
-      <c r="DU1" s="1"/>
-      <c r="DV1" s="1"/>
-      <c r="DW1" s="1"/>
-      <c r="DX1" s="1"/>
-      <c r="DY1" s="1"/>
-      <c r="DZ1" s="1"/>
-      <c r="EA1" s="1"/>
-      <c r="EB1" s="1"/>
-      <c r="EC1" s="1"/>
-      <c r="ED1" s="1"/>
-      <c r="EE1" s="1"/>
-      <c r="EF1" s="1"/>
-      <c r="EG1" s="1"/>
-      <c r="EH1" s="1"/>
-      <c r="EI1" s="1"/>
-      <c r="EJ1" s="1"/>
-      <c r="EK1" s="1"/>
-      <c r="EL1" s="1"/>
-      <c r="EM1" s="1"/>
-      <c r="EN1" s="1"/>
-      <c r="EO1" s="1"/>
-      <c r="EP1" s="1"/>
-      <c r="EQ1" s="1"/>
-      <c r="ER1" s="1"/>
-      <c r="ES1" s="1"/>
-      <c r="ET1" s="1"/>
-      <c r="EU1" s="1"/>
-      <c r="EV1" s="1"/>
-      <c r="EW1" s="1"/>
-      <c r="EX1" s="1"/>
-      <c r="EY1" s="1"/>
-      <c r="EZ1" s="1"/>
-      <c r="FA1" s="1"/>
-      <c r="FB1" s="1"/>
-      <c r="FC1" s="1"/>
-      <c r="FD1" s="1"/>
-      <c r="FE1" s="1"/>
-      <c r="FF1" s="1"/>
-      <c r="FG1" s="1"/>
-      <c r="FH1" s="1"/>
-      <c r="FI1" s="1"/>
-      <c r="FJ1" s="1"/>
-      <c r="FK1" s="1"/>
-      <c r="FL1" s="1"/>
-      <c r="FM1" s="1"/>
-      <c r="FN1" s="1"/>
-      <c r="FO1" s="1"/>
-      <c r="FP1" s="1"/>
-      <c r="FQ1" s="1"/>
-      <c r="FR1" s="1"/>
-      <c r="FS1" s="1"/>
-      <c r="FT1" s="1"/>
-      <c r="FU1" s="1"/>
-      <c r="FV1" s="1"/>
-      <c r="FW1" s="1"/>
-      <c r="FX1" s="1"/>
-      <c r="FY1" s="1"/>
-      <c r="FZ1" s="1"/>
-      <c r="GA1" s="1"/>
-      <c r="GB1" s="1"/>
-      <c r="GC1" s="1"/>
-      <c r="GD1" s="1"/>
-      <c r="GE1" s="1"/>
-      <c r="GF1" s="1"/>
-      <c r="GG1" s="1"/>
-      <c r="GH1" s="1"/>
-      <c r="GI1" s="1"/>
-      <c r="GJ1" s="1"/>
-      <c r="GK1" s="1"/>
-      <c r="GL1" s="1"/>
-      <c r="GM1" s="1"/>
-      <c r="GN1" s="1"/>
-      <c r="GO1" s="1"/>
-      <c r="GP1" s="1"/>
-      <c r="GQ1" s="1"/>
-      <c r="GR1" s="1"/>
-      <c r="GS1" s="1"/>
-      <c r="GT1" s="1"/>
-      <c r="GU1" s="1"/>
-      <c r="GV1" s="1"/>
-      <c r="GW1" s="1"/>
-      <c r="GX1" s="1"/>
-      <c r="GY1" s="1"/>
-      <c r="GZ1" s="1"/>
-      <c r="HA1" s="1"/>
-      <c r="HB1" s="1"/>
-      <c r="HC1" s="1"/>
-      <c r="HD1" s="1"/>
-      <c r="HE1" s="1"/>
-      <c r="HF1" s="1"/>
-      <c r="HG1" s="1"/>
-      <c r="HH1" s="1"/>
-      <c r="HI1" s="1"/>
-      <c r="HJ1" s="1"/>
-      <c r="HK1" s="1"/>
-      <c r="HL1" s="1"/>
-      <c r="HM1" s="1"/>
-      <c r="HN1" s="1"/>
-      <c r="HO1" s="1"/>
-      <c r="HP1" s="1"/>
-      <c r="HQ1" s="1"/>
-      <c r="HR1" s="1"/>
-      <c r="HS1" s="1"/>
-      <c r="HT1" s="1"/>
-      <c r="HU1" s="1"/>
-      <c r="HV1" s="1"/>
-      <c r="HW1" s="1"/>
-      <c r="HX1" s="1"/>
-      <c r="HY1" s="1"/>
-      <c r="HZ1" s="1"/>
-      <c r="IA1" s="1"/>
-      <c r="IB1" s="1"/>
-      <c r="IC1" s="1"/>
-      <c r="ID1" s="1"/>
-      <c r="IE1" s="1"/>
-      <c r="IF1" s="1"/>
-      <c r="IG1" s="1"/>
-      <c r="IH1" s="1"/>
-      <c r="II1" s="1"/>
-      <c r="IJ1" s="1"/>
-      <c r="IK1" s="1"/>
-      <c r="IL1" s="1"/>
-      <c r="IM1" s="1"/>
-      <c r="IN1" s="1"/>
-      <c r="IO1" s="1"/>
-      <c r="IP1" s="1"/>
-      <c r="IQ1" s="1"/>
-      <c r="IR1" s="1"/>
-      <c r="IS1" s="1"/>
-      <c r="IT1" s="1"/>
-      <c r="IU1" s="1"/>
-      <c r="IV1" s="1"/>
-    </row>
-    <row r="2" ht="15.75" spans="2:11">
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="65" t="s">
+      <c r="J2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="76" t="s">
+      <c r="K2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="66" t="s">
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="47" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="68"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="69"/>
+    </row>
+    <row r="4" ht="15.75" spans="2:11">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80"/>
+    </row>
+    <row r="5" ht="15.75" spans="2:11">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="68"/>
-    </row>
-    <row r="4" ht="15.75" spans="2:11">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" ht="15.75" spans="2:11">
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="21" spans="2:11">
+      <c r="B6" s="9">
+        <v>2025</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="80" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="21" spans="2:11">
-      <c r="B6" s="8">
-        <v>2025</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="82"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="C7" s="12">
         <v>202</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="13">
         <v>121</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="52">
         <v>77</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="53">
         <v>6</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="83">
+      <c r="G7" s="12"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="84">
         <v>406</v>
       </c>
-      <c r="J7" s="84">
+      <c r="J7" s="85">
         <f>I7/$I$19</f>
         <v>0.559228650137741</v>
       </c>
-      <c r="K7" s="85" t="s">
-        <v>19</v>
+      <c r="K7" s="86" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
         <v>202</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="16">
         <v>285</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="54">
         <v>426</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="55">
         <v>82</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="86">
+      <c r="G8" s="15"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="87">
         <v>995</v>
       </c>
-      <c r="J8" s="87">
+      <c r="J8" s="88">
         <f>I8/$I$20</f>
         <v>0.196640316205534</v>
       </c>
-      <c r="K8" s="88" t="s">
-        <v>20</v>
+      <c r="K8" s="89" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="13"/>
-      <c r="C9" s="16">
+      <c r="B9" s="14"/>
+      <c r="C9" s="17">
         <v>5768349.4</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="18">
         <v>6817663.4</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="56">
         <v>5687694.82</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="57">
         <v>446821.7</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="89">
+      <c r="G9" s="58"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="90">
         <v>18720529.32</v>
       </c>
-      <c r="J9" s="90">
+      <c r="J9" s="91">
         <f>I9/$I$21</f>
         <v>0.051788408995017</v>
       </c>
-      <c r="K9" s="88" t="s">
-        <v>21</v>
+      <c r="K9" s="89" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="13"/>
-      <c r="C10" s="18">
+      <c r="B10" s="14"/>
+      <c r="C10" s="19">
         <v>28556.19</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="18">
         <v>23921.63</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="56">
         <v>13351.4</v>
       </c>
-      <c r="F10" s="56">
+      <c r="F10" s="57">
         <v>5449.05</v>
       </c>
-      <c r="G10" s="57"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="89">
+      <c r="G10" s="58"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="90">
         <v>17819.57</v>
       </c>
-      <c r="J10" s="90">
+      <c r="J10" s="91">
         <f>I10/$I$28</f>
         <v>0.0759846730147153</v>
       </c>
-      <c r="K10" s="88" t="s">
+      <c r="K10" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="2:11">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21">
+        <v>30.81</v>
+      </c>
+      <c r="D11" s="22">
+        <v>36.42</v>
+      </c>
+      <c r="E11" s="60">
+        <v>30.38</v>
+      </c>
+      <c r="F11" s="61">
+        <v>2.39</v>
+      </c>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="92">
+        <v>100</v>
+      </c>
+      <c r="J11" s="93"/>
+      <c r="K11" s="94" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" ht="15.75" spans="2:11">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20">
+    <row r="12" ht="9" customHeight="1" spans="2:11">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24">
         <v>30.81</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D12" s="24">
         <v>36.42</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E12" s="24">
         <v>30.38</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F12" s="24">
         <v>2.39</v>
       </c>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="91">
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24">
         <v>100</v>
       </c>
-      <c r="J11" s="92"/>
-      <c r="K11" s="93" t="s">
+      <c r="J12" s="24"/>
+      <c r="K12" s="95"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" ht="9" customHeight="1" spans="2:11">
-      <c r="B12" s="22"/>
-      <c r="C12" s="23">
-        <v>30.81</v>
-      </c>
-      <c r="D12" s="23">
-        <v>36.42</v>
-      </c>
-      <c r="E12" s="23">
-        <v>30.38</v>
-      </c>
-      <c r="F12" s="23">
-        <v>2.39</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23">
-        <v>100</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="94"/>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="11">
+      <c r="C13" s="12">
         <v>26</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="13">
         <v>52</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="12">
         <v>126</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="13">
         <v>103</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="52">
         <v>13</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="83">
+      <c r="H13" s="53"/>
+      <c r="I13" s="84">
         <v>320</v>
       </c>
-      <c r="J13" s="84">
+      <c r="J13" s="85">
         <f>I13/$I$19</f>
         <v>0.440771349862259</v>
       </c>
-      <c r="K13" s="85" t="s">
-        <v>19</v>
+      <c r="K13" s="86" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="25"/>
-      <c r="C14" s="14">
+      <c r="B14" s="26"/>
+      <c r="C14" s="15">
         <v>26</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="16">
         <v>131</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="15">
         <v>814</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="16">
         <v>2174</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="54">
         <v>920</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="86">
+      <c r="H14" s="55"/>
+      <c r="I14" s="87">
         <v>4065</v>
       </c>
-      <c r="J14" s="87">
+      <c r="J14" s="88">
         <f>I14/$I$20</f>
         <v>0.803359683794466</v>
       </c>
-      <c r="K14" s="88" t="s">
-        <v>25</v>
+      <c r="K14" s="89" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="25"/>
-      <c r="C15" s="16">
+      <c r="B15" s="26"/>
+      <c r="C15" s="17">
         <v>11818125.9</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="18">
         <v>23311544.65</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="19">
         <v>99037537.05</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="18">
         <v>150010744.56</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="56">
         <v>58582585.1</v>
       </c>
-      <c r="H15" s="56"/>
-      <c r="I15" s="89">
+      <c r="H15" s="57"/>
+      <c r="I15" s="90">
         <v>342760537.26</v>
       </c>
-      <c r="J15" s="90">
+      <c r="J15" s="91">
         <f>I15/$I$21</f>
         <v>0.948211591004983</v>
       </c>
-      <c r="K15" s="88" t="s">
-        <v>21</v>
+      <c r="K15" s="89" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="25"/>
-      <c r="C16" s="18">
+      <c r="B16" s="26"/>
+      <c r="C16" s="19">
         <v>454543.3</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="18">
         <v>177950.72</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="19">
         <v>121667.74</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="18">
         <v>69002.18</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16" s="56">
         <v>63676.72</v>
       </c>
-      <c r="H16" s="56"/>
-      <c r="I16" s="95">
+      <c r="H16" s="57"/>
+      <c r="I16" s="96">
         <v>177368.13</v>
       </c>
-      <c r="J16" s="90">
+      <c r="J16" s="91">
         <f>I16/$I$28</f>
         <v>0.756317877551563</v>
       </c>
-      <c r="K16" s="88" t="s">
+      <c r="K16" s="89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="2:11">
+      <c r="B17" s="27"/>
+      <c r="C17" s="21">
+        <v>3.45</v>
+      </c>
+      <c r="D17" s="22">
+        <v>6.8</v>
+      </c>
+      <c r="E17" s="21">
+        <v>28.89</v>
+      </c>
+      <c r="F17" s="22">
+        <v>43.77</v>
+      </c>
+      <c r="G17" s="60">
+        <v>17.09</v>
+      </c>
+      <c r="H17" s="61"/>
+      <c r="I17" s="92">
+        <v>100</v>
+      </c>
+      <c r="J17" s="93"/>
+      <c r="K17" s="94" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="2:11">
-      <c r="B17" s="26"/>
-      <c r="C17" s="20">
+    <row r="18" ht="9" customHeight="1" spans="2:11">
+      <c r="B18" s="23"/>
+      <c r="C18" s="24">
         <v>3.45</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D18" s="24">
         <v>6.8</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="24">
         <v>28.89</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F18" s="24">
         <v>43.77</v>
       </c>
-      <c r="G17" s="59">
+      <c r="G18" s="24">
         <v>17.09</v>
       </c>
-      <c r="H17" s="60"/>
-      <c r="I17" s="91">
+      <c r="H18" s="24"/>
+      <c r="I18" s="24">
         <v>100</v>
       </c>
-      <c r="J17" s="92"/>
-      <c r="K17" s="93" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" ht="9" customHeight="1" spans="2:11">
-      <c r="B18" s="22"/>
-      <c r="C18" s="23">
-        <v>3.45</v>
-      </c>
-      <c r="D18" s="23">
-        <v>6.8</v>
-      </c>
-      <c r="E18" s="23">
-        <v>28.89</v>
-      </c>
-      <c r="F18" s="23">
-        <v>43.77</v>
-      </c>
-      <c r="G18" s="23">
-        <v>17.09</v>
-      </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23">
-        <v>100</v>
-      </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="94"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="95"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="12">
         <v>228</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="13">
         <v>173</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="52">
         <v>203</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="53">
         <v>109</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="12">
         <v>13</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="13">
         <f t="shared" ref="C19:I19" si="0">H7+H13</f>
         <v>0</v>
       </c>
-      <c r="I19" s="96">
+      <c r="I19" s="97">
         <v>726</v>
       </c>
-      <c r="J19" s="97">
+      <c r="J19" s="98">
         <v>1</v>
       </c>
-      <c r="K19" s="98" t="s">
-        <v>19</v>
+      <c r="K19" s="99" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="28"/>
-      <c r="C20" s="14">
+      <c r="B20" s="29"/>
+      <c r="C20" s="15">
         <v>228</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="16">
         <v>416</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="54">
         <v>1240</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="55">
         <v>2256</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="15">
         <v>920</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="16">
         <f t="shared" ref="C20:I20" si="1">H8+H14</f>
         <v>0</v>
       </c>
-      <c r="I20" s="99">
+      <c r="I20" s="100">
         <v>5060</v>
       </c>
-      <c r="J20" s="100">
+      <c r="J20" s="101">
         <v>1</v>
       </c>
-      <c r="K20" s="101" t="s">
-        <v>25</v>
+      <c r="K20" s="102" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="28"/>
-      <c r="C21" s="16">
+      <c r="B21" s="29"/>
+      <c r="C21" s="17">
         <v>17586475.3</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="18">
         <v>30129208.05</v>
       </c>
-      <c r="E21" s="55">
+      <c r="E21" s="56">
         <v>104725231.87</v>
       </c>
-      <c r="F21" s="56">
+      <c r="F21" s="57">
         <v>150457566.26</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="19">
         <v>58582585.1</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="18">
         <f t="shared" ref="C21:H21" si="2">H9+H15</f>
         <v>0</v>
       </c>
-      <c r="I21" s="102">
+      <c r="I21" s="103">
         <v>361481066.58</v>
       </c>
-      <c r="J21" s="103">
+      <c r="J21" s="104">
         <v>1</v>
       </c>
-      <c r="K21" s="101" t="s">
-        <v>21</v>
+      <c r="K21" s="102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="28"/>
-      <c r="C22" s="18">
+      <c r="B22" s="29"/>
+      <c r="C22" s="19">
         <v>77133.66</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="18">
         <v>72425.98</v>
       </c>
-      <c r="E22" s="55">
+      <c r="E22" s="56">
         <v>84455.83</v>
       </c>
-      <c r="F22" s="56">
+      <c r="F22" s="57">
         <v>66692.18</v>
       </c>
-      <c r="G22" s="63">
+      <c r="G22" s="64">
         <v>63676.72</v>
       </c>
-      <c r="H22" s="64" t="e">
-        <f t="shared" ref="C22:H22" si="3">H21/H20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="104">
+      <c r="H22" s="65">
+        <v>0</v>
+      </c>
+      <c r="I22" s="105">
         <v>72876.87</v>
       </c>
-      <c r="J22" s="90">
+      <c r="J22" s="91">
         <f>I22/I28</f>
         <v>0.310755261618878</v>
       </c>
-      <c r="K22" s="101" t="s">
+      <c r="K22" s="102" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="2:11">
+      <c r="B23" s="30"/>
+      <c r="C23" s="21">
+        <v>4.87</v>
+      </c>
+      <c r="D23" s="22">
+        <v>8.33</v>
+      </c>
+      <c r="E23" s="60">
+        <v>28.97</v>
+      </c>
+      <c r="F23" s="61">
+        <v>41.62</v>
+      </c>
+      <c r="G23" s="21">
+        <v>16.21</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" ref="C23:H23" si="3">H21/$I$21</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="106">
+        <v>100</v>
+      </c>
+      <c r="J23" s="93"/>
+      <c r="K23" s="107" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" ht="15.75" spans="2:11">
-      <c r="B23" s="29"/>
-      <c r="C23" s="20">
+    <row r="24" ht="9" customHeight="1" spans="2:11">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32">
         <v>4.87</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D24" s="32">
         <v>8.33</v>
       </c>
-      <c r="E23" s="59">
+      <c r="E24" s="32">
         <v>28.97</v>
       </c>
-      <c r="F23" s="60">
+      <c r="F24" s="32">
         <v>41.62</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G24" s="32">
         <v>16.21</v>
       </c>
-      <c r="H23" s="21">
-        <f t="shared" ref="C23:H23" si="4">H21/$I$21</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="105">
+      <c r="H24" s="32"/>
+      <c r="I24" s="32">
         <v>100</v>
       </c>
-      <c r="J23" s="92"/>
-      <c r="K23" s="106" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" ht="9" customHeight="1" spans="2:11">
-      <c r="B24" s="30"/>
-      <c r="C24" s="31">
-        <v>4.87</v>
-      </c>
-      <c r="D24" s="31">
-        <v>8.33</v>
-      </c>
-      <c r="E24" s="31">
-        <v>28.97</v>
-      </c>
-      <c r="F24" s="31">
-        <v>41.62</v>
-      </c>
-      <c r="G24" s="31">
-        <v>16.21</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31">
-        <v>100</v>
-      </c>
-      <c r="J24" s="31"/>
-      <c r="K24" s="107"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="108"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="11">
+      <c r="B25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="12">
         <f>C13</f>
         <v>26</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="13">
         <f>D13</f>
         <v>52</v>
       </c>
-      <c r="E25" s="65">
+      <c r="E25" s="66">
         <f>SUM(E19:H19)</f>
         <v>325</v>
       </c>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="96">
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="97">
         <f>SUM(C25:H25)</f>
         <v>403</v>
       </c>
-      <c r="J25" s="108">
+      <c r="J25" s="109">
         <f>I25/I19</f>
         <v>0.555096418732782</v>
       </c>
-      <c r="K25" s="98" t="s">
-        <v>19</v>
+      <c r="K25" s="99" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="13"/>
-      <c r="C26" s="14">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15">
         <v>0</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="16">
         <v>0</v>
       </c>
-      <c r="E26" s="67">
+      <c r="E26" s="68">
         <f>SUM(E20:H20)</f>
         <v>4416</v>
       </c>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="99">
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="100">
         <f>SUM(C26:H26)</f>
         <v>4416</v>
       </c>
-      <c r="J26" s="87">
+      <c r="J26" s="88">
         <f>I26/I20</f>
         <v>0.872727272727273</v>
       </c>
-      <c r="K26" s="101" t="s">
-        <v>25</v>
+      <c r="K26" s="102" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="13"/>
-      <c r="C27" s="18">
+      <c r="B27" s="14"/>
+      <c r="C27" s="19">
         <f>C15</f>
         <v>11818125.9</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="18">
         <f>D15</f>
         <v>23311544.65</v>
       </c>
-      <c r="E27" s="69">
+      <c r="E27" s="70">
         <f>SUM(E21:H21)</f>
         <v>313765383.23</v>
       </c>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="102">
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="103">
         <f>SUM(C27:H27)</f>
         <v>348895053.78</v>
       </c>
-      <c r="J27" s="90">
+      <c r="J27" s="91">
         <f>I27/I21</f>
         <v>0.965182096757993</v>
       </c>
-      <c r="K27" s="101" t="s">
-        <v>21</v>
+      <c r="K27" s="102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="13"/>
-      <c r="C28" s="18">
+      <c r="B28" s="14"/>
+      <c r="C28" s="19">
         <f>C16</f>
         <v>454543.3</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="18">
         <f>D16</f>
         <v>177950.72</v>
       </c>
-      <c r="E28" s="69">
+      <c r="E28" s="70">
         <f>E27/E26</f>
         <v>71051.9436662138</v>
       </c>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="104">
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="105">
         <f>AVERAGE(C28:H28)</f>
         <v>234515.321222071</v>
       </c>
-      <c r="J28" s="103">
+      <c r="J28" s="104">
         <v>1</v>
       </c>
-      <c r="K28" s="101" t="s">
-        <v>22</v>
+      <c r="K28" s="102" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" ht="15.75" spans="2:11">
-      <c r="B29" s="19"/>
-      <c r="C29" s="32">
+      <c r="B29" s="20"/>
+      <c r="C29" s="33">
         <f>C27/I27</f>
         <v>0.0338730107290431</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="34">
         <f>D27/I27</f>
         <v>0.0668153486197009</v>
       </c>
-      <c r="E29" s="71">
+      <c r="E29" s="72">
         <f>E27/I27</f>
         <v>0.899311640651256</v>
       </c>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="109">
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="110">
         <v>1</v>
       </c>
-      <c r="J29" s="92"/>
-      <c r="K29" s="106" t="s">
-        <v>23</v>
+      <c r="J29" s="93"/>
+      <c r="K29" s="107" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" ht="15.75"/>
     <row r="31" spans="2:11">
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="D31" s="36"/>
+      <c r="E31" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="74" t="s">
+      <c r="F31" s="75"/>
+      <c r="G31" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="74"/>
-      <c r="G31" s="34" t="s">
+      <c r="H31" s="36"/>
+      <c r="I31" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="H31" s="35"/>
-      <c r="I31" s="74" t="s">
+      <c r="J31" s="75"/>
+      <c r="K31" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="74"/>
-      <c r="K31" s="110" t="s">
+    </row>
+    <row r="32" ht="15.75" spans="2:11">
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="112"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" spans="2:11">
+      <c r="B33" s="39" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" spans="2:11">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="111"/>
-    </row>
-    <row r="33" ht="18" customHeight="1" spans="2:11">
-      <c r="B33" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="39">
+      <c r="C33" s="40">
         <f>C7+D7</f>
         <v>323</v>
       </c>
-      <c r="D33" s="40"/>
-      <c r="E33" s="39">
+      <c r="D33" s="41"/>
+      <c r="E33" s="40">
         <f>C13</f>
         <v>26</v>
       </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="39">
+      <c r="F33" s="41"/>
+      <c r="G33" s="40">
         <f>D13</f>
         <v>52</v>
       </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="39">
+      <c r="H33" s="41"/>
+      <c r="I33" s="40">
         <f>E25</f>
         <v>325</v>
       </c>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40">
+      <c r="J33" s="41"/>
+      <c r="K33" s="41">
         <f>C33+E33+G33+I33</f>
         <v>726</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1" spans="2:11">
-      <c r="B34" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="42">
+      <c r="B34" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="43">
         <f>C33/$K$33</f>
         <v>0.444903581267218</v>
       </c>
-      <c r="D34" s="43"/>
-      <c r="E34" s="42">
+      <c r="D34" s="44"/>
+      <c r="E34" s="43">
         <f>E33/$K$33</f>
         <v>0.0358126721763085</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="42">
+      <c r="F34" s="44"/>
+      <c r="G34" s="43">
         <f>G33/$K$33</f>
         <v>0.0716253443526171</v>
       </c>
-      <c r="H34" s="43"/>
-      <c r="I34" s="42">
+      <c r="H34" s="44"/>
+      <c r="I34" s="43">
         <f>I33/$K$33</f>
         <v>0.447658402203857</v>
       </c>
-      <c r="J34" s="43"/>
-      <c r="K34" s="112">
+      <c r="J34" s="44"/>
+      <c r="K34" s="113">
         <v>1</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" spans="2:11">
-      <c r="B35" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="39">
+      <c r="B35" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="40">
         <f>C9+D9</f>
         <v>12586012.8</v>
       </c>
-      <c r="D35" s="40"/>
-      <c r="E35" s="39">
+      <c r="D35" s="41"/>
+      <c r="E35" s="40">
         <f>C15</f>
         <v>11818125.9</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="39">
+      <c r="F35" s="41"/>
+      <c r="G35" s="40">
         <f>D15</f>
         <v>23311544.65</v>
       </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="39">
+      <c r="H35" s="41"/>
+      <c r="I35" s="40">
         <f>E27</f>
         <v>313765383.23</v>
       </c>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40">
+      <c r="J35" s="41"/>
+      <c r="K35" s="41">
         <f>C35+E35+G35+I35</f>
         <v>361481066.58</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="2:11">
-      <c r="B36" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="42">
+      <c r="B36" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="43">
         <f>C35/$K$35</f>
         <v>0.0348179032420072</v>
       </c>
-      <c r="D36" s="43"/>
-      <c r="E36" s="42">
+      <c r="D36" s="44"/>
+      <c r="E36" s="43">
         <f>E35/$K$35</f>
         <v>0.0326936235189638</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="42">
+      <c r="F36" s="44"/>
+      <c r="G36" s="43">
         <f>G35/$K$35</f>
         <v>0.0644889782763792</v>
       </c>
-      <c r="H36" s="43"/>
-      <c r="I36" s="42">
+      <c r="H36" s="44"/>
+      <c r="I36" s="43">
         <f>I35/$K$35</f>
         <v>0.86799949496265</v>
       </c>
-      <c r="J36" s="43"/>
-      <c r="K36" s="112">
+      <c r="J36" s="44"/>
+      <c r="K36" s="113">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="A1:IV1"/>
+  <mergeCells count="46">
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B12:K12"/>

</xml_diff>